<commit_message>
temp commit by windows
</commit_message>
<xml_diff>
--- a/data/Output/かこい屋/店舗情報まとめ.xlsx
+++ b/data/Output/かこい屋/店舗情報まとめ.xlsx
@@ -1599,7 +1599,7 @@
         <v>6026.517241379311</v>
       </c>
       <c r="H2" t="n">
-        <v>961229.5</v>
+        <v>3013.258620689655</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1625,7 +1625,7 @@
         <v>8846.896551724138</v>
       </c>
       <c r="H3" t="n">
-        <v>598640</v>
+        <v>2948.965517241379</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1651,7 +1651,7 @@
         <v>11520.87837837838</v>
       </c>
       <c r="H4" t="n">
-        <v>426272.5</v>
+        <v>2880.219594594595</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1677,7 +1677,7 @@
         <v>6559.789473684211</v>
       </c>
       <c r="H5" t="n">
-        <v>311590</v>
+        <v>3279.894736842105</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1703,7 +1703,7 @@
         <v>5224.193548387097</v>
       </c>
       <c r="H6" t="n">
-        <v>242925</v>
+        <v>2612.096774193548</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1755,7 +1755,7 @@
         <v>13385.43835616438</v>
       </c>
       <c r="H8" t="n">
-        <v>195427.4</v>
+        <v>2677.087671232877</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1781,7 +1781,7 @@
         <v>17103.6</v>
       </c>
       <c r="H9" t="n">
-        <v>142530</v>
+        <v>2850.6</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1807,7 +1807,7 @@
         <v>11646.875</v>
       </c>
       <c r="H10" t="n">
-        <v>93175</v>
+        <v>2911.71875</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1833,7 +1833,7 @@
         <v>7930.9375</v>
       </c>
       <c r="H11" t="n">
-        <v>84596.66666666667</v>
+        <v>2643.645833333333</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1859,7 +1859,7 @@
         <v>23549.03225806452</v>
       </c>
       <c r="H12" t="n">
-        <v>91252.5</v>
+        <v>2943.629032258064</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1885,7 +1885,7 @@
         <v>17104.16666666667</v>
       </c>
       <c r="H13" t="n">
-        <v>58642.85714285714</v>
+        <v>2443.452380952381</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1911,7 +1911,7 @@
         <v>9711.818181818182</v>
       </c>
       <c r="H14" t="n">
-        <v>53415</v>
+        <v>2427.954545454545</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1937,7 +1937,7 @@
         <v>8198.5</v>
       </c>
       <c r="H15" t="n">
-        <v>54656.66666666666</v>
+        <v>2732.833333333333</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1963,7 +1963,7 @@
         <v>24522.22222222222</v>
       </c>
       <c r="H16" t="n">
-        <v>49044.44444444445</v>
+        <v>2724.691358024691</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1989,7 +1989,7 @@
         <v>26929.33333333333</v>
       </c>
       <c r="H17" t="n">
-        <v>40394</v>
+        <v>2692.933333333333</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2015,7 +2015,7 @@
         <v>36722.85714285714</v>
       </c>
       <c r="H18" t="n">
-        <v>46738.18181818182</v>
+        <v>3338.441558441559</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2041,7 +2041,7 @@
         <v>13569.16666666667</v>
       </c>
       <c r="H19" t="n">
-        <v>32566</v>
+        <v>2713.833333333333</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2067,7 +2067,7 @@
         <v>8780</v>
       </c>
       <c r="H20" t="n">
-        <v>32193.33333333333</v>
+        <v>2926.666666666667</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2093,7 +2093,7 @@
         <v>34210</v>
       </c>
       <c r="H21" t="n">
-        <v>31359.16666666667</v>
+        <v>2850.833333333333</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2119,7 +2119,7 @@
         <v>3986.25</v>
       </c>
       <c r="H22" t="n">
-        <v>31890</v>
+        <v>3986.25</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2145,7 +2145,7 @@
         <v>55172.5</v>
       </c>
       <c r="H23" t="n">
-        <v>27586.25</v>
+        <v>3448.28125</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2171,7 +2171,7 @@
         <v>44312.5</v>
       </c>
       <c r="H24" t="n">
-        <v>27269.23076923077</v>
+        <v>3408.653846153846</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2197,7 +2197,7 @@
         <v>48791.42857142857</v>
       </c>
       <c r="H25" t="n">
-        <v>22769.33333333333</v>
+        <v>3252.761904761905</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2223,7 +2223,7 @@
         <v>8400</v>
       </c>
       <c r="H26" t="n">
-        <v>14700</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2249,7 +2249,7 @@
         <v>11032.85714285714</v>
       </c>
       <c r="H27" t="n">
-        <v>15446</v>
+        <v>2206.571428571428</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2275,7 +2275,7 @@
         <v>37855.71428571428</v>
       </c>
       <c r="H28" t="n">
-        <v>18927.85714285714</v>
+        <v>2703.979591836734</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2301,7 +2301,7 @@
         <v>14937.14285714286</v>
       </c>
       <c r="H29" t="n">
-        <v>17426.66666666667</v>
+        <v>2489.52380952381</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2327,7 +2327,7 @@
         <v>23640</v>
       </c>
       <c r="H30" t="n">
-        <v>17730</v>
+        <v>2955</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2353,7 +2353,7 @@
         <v>66120</v>
       </c>
       <c r="H31" t="n">
-        <v>14693.33333333333</v>
+        <v>3673.333333333333</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2379,7 +2379,7 @@
         <v>73465</v>
       </c>
       <c r="H32" t="n">
-        <v>15466.31578947369</v>
+        <v>3866.578947368421</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2405,7 +2405,7 @@
         <v>26752.5</v>
       </c>
       <c r="H33" t="n">
-        <v>10701</v>
+        <v>2675.25</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2431,7 +2431,7 @@
         <v>64920</v>
       </c>
       <c r="H34" t="n">
-        <v>12984</v>
+        <v>3246</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2457,7 +2457,7 @@
         <v>97680</v>
       </c>
       <c r="H35" t="n">
-        <v>11721.6</v>
+        <v>3907.2</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2483,7 +2483,7 @@
         <v>74820</v>
       </c>
       <c r="H36" t="n">
-        <v>6506.086956521739</v>
+        <v>3253.04347826087</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2509,7 +2509,7 @@
         <v>9850</v>
       </c>
       <c r="H37" t="n">
-        <v>3940</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2535,7 +2535,7 @@
         <v>113690</v>
       </c>
       <c r="H38" t="n">
-        <v>8120.714285714285</v>
+        <v>4060.357142857143</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2561,7 +2561,7 @@
         <v>37000</v>
       </c>
       <c r="H39" t="n">
-        <v>2055.555555555556</v>
+        <v>1027.777777777778</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2587,7 +2587,7 @@
         <v>31000</v>
       </c>
       <c r="H40" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2613,7 +2613,7 @@
         <v>74090</v>
       </c>
       <c r="H41" t="n">
-        <v>8716.470588235294</v>
+        <v>4358.235294117647</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2639,7 +2639,7 @@
         <v>21310</v>
       </c>
       <c r="H42" t="n">
-        <v>6088.571428571428</v>
+        <v>3044.285714285714</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2665,7 +2665,7 @@
         <v>10800</v>
       </c>
       <c r="H43" t="n">
-        <v>3600</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2691,7 +2691,7 @@
         <v>26120</v>
       </c>
       <c r="H44" t="n">
-        <v>4353.333333333333</v>
+        <v>2176.666666666667</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2717,7 +2717,7 @@
         <v>29430</v>
       </c>
       <c r="H45" t="n">
-        <v>6540</v>
+        <v>3270</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2743,7 +2743,7 @@
         <v>-6615</v>
       </c>
       <c r="H46" t="n">
-        <v>6615</v>
+        <v>3307.5</v>
       </c>
     </row>
     <row r="47" spans="1:8">

</xml_diff>